<commit_message>
fin import et tdb généraux
</commit_message>
<xml_diff>
--- a/demos/structures.xlsx
+++ b/demos/structures.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25320" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="19320" windowHeight="12120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">structure!$A$1:$AMK$159</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">structure!$A$1:$AMK$160</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="577">
   <si>
     <t>nofiness</t>
   </si>
@@ -1668,9 +1668,6 @@
     <t>Réanimation médicale</t>
   </si>
   <si>
-    <t>Gériarie</t>
-  </si>
-  <si>
     <t>Hématologie Clinique</t>
   </si>
   <si>
@@ -1738,6 +1735,24 @@
   </si>
   <si>
     <t>ORL SLS</t>
+  </si>
+  <si>
+    <t>Gériatrie</t>
+  </si>
+  <si>
+    <t>2669</t>
+  </si>
+  <si>
+    <t>095J</t>
+  </si>
+  <si>
+    <t>76095J</t>
+  </si>
+  <si>
+    <t>PHARMACO CLI HDJ</t>
+  </si>
+  <si>
+    <t>Pharmacologie clinique</t>
   </si>
 </sst>
 </file>
@@ -2081,10 +2096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK159"/>
+  <dimension ref="A1:AMK160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F155" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,7 +2247,7 @@
         <v>113</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>114</v>
@@ -2261,7 +2276,7 @@
         <v>117</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>114</v>
@@ -2290,7 +2305,7 @@
         <v>120</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>114</v>
@@ -2319,7 +2334,7 @@
         <v>124</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>114</v>
@@ -2348,10 +2363,10 @@
         <v>67</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>35</v>
@@ -2377,10 +2392,10 @@
         <v>67</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>35</v>
@@ -2406,10 +2421,10 @@
         <v>67</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>35</v>
@@ -2435,10 +2450,10 @@
         <v>67</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>35</v>
@@ -2464,10 +2479,10 @@
         <v>67</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>35</v>
@@ -2493,10 +2508,10 @@
         <v>67</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>35</v>
@@ -2522,10 +2537,10 @@
         <v>67</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>35</v>
@@ -2812,7 +2827,7 @@
         <v>79</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>76</v>
@@ -3192,7 +3207,7 @@
         <v>525</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>137</v>
@@ -3221,7 +3236,7 @@
         <v>525</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>137</v>
@@ -3250,7 +3265,7 @@
         <v>525</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>137</v>
@@ -3496,7 +3511,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>396</v>
@@ -3769,10 +3784,10 @@
         <v>265</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>54</v>
@@ -3798,10 +3813,10 @@
         <v>268</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>54</v>
@@ -3827,10 +3842,10 @@
         <v>265</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>54</v>
@@ -3943,10 +3958,10 @@
         <v>461</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>54</v>
@@ -3972,10 +3987,10 @@
         <v>465</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>54</v>
@@ -4001,7 +4016,7 @@
         <v>203</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>204</v>
@@ -4030,7 +4045,7 @@
         <v>207</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>203</v>
@@ -4059,7 +4074,7 @@
         <v>203</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>204</v>
@@ -4233,10 +4248,10 @@
         <v>244</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>54</v>
@@ -4262,10 +4277,10 @@
         <v>247</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>54</v>
@@ -4291,10 +4306,10 @@
         <v>244</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>54</v>
@@ -4320,10 +4335,10 @@
         <v>262</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>54</v>
@@ -4349,10 +4364,10 @@
         <v>253</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>54</v>
@@ -4378,10 +4393,10 @@
         <v>256</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>54</v>
@@ -4407,10 +4422,10 @@
         <v>253</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>54</v>
@@ -4766,31 +4781,31 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>750100042</v>
+        <v>750100075</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C92" s="1">
-        <v>2297</v>
+        <v>19</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>572</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>531</v>
+        <v>573</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>532</v>
+        <v>574</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>533</v>
+        <v>575</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>555</v>
+        <v>576</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>555</v>
+        <v>576</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4801,22 +4816,22 @@
         <v>9</v>
       </c>
       <c r="C93" s="1">
-        <v>2299</v>
+        <v>2297</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>15</v>
@@ -4830,22 +4845,22 @@
         <v>9</v>
       </c>
       <c r="C94" s="1">
-        <v>2450</v>
+        <v>2299</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>15</v>
@@ -4853,28 +4868,28 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>750100075</v>
+        <v>750100042</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2450</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>11</v>
+        <v>537</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>12</v>
+        <v>538</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>13</v>
+        <v>539</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>14</v>
+        <v>554</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>14</v>
+        <v>554</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>15</v>
@@ -4887,17 +4902,17 @@
       <c r="B96" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C96" s="1">
-        <v>1019</v>
+      <c r="C96" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>14</v>
@@ -4911,28 +4926,28 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>750100042</v>
+        <v>750100075</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C97" s="1">
-        <v>1366</v>
+        <v>1019</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>216</v>
+        <v>16</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>513</v>
+        <v>17</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>514</v>
+        <v>18</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>548</v>
+        <v>14</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>548</v>
+        <v>14</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>15</v>
@@ -4945,23 +4960,23 @@
       <c r="B98" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>515</v>
+      <c r="C98" s="1">
+        <v>1366</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>516</v>
+        <v>216</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>548</v>
+        <v>571</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>548</v>
+        <v>571</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>15</v>
@@ -4974,23 +4989,23 @@
       <c r="B99" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C99" s="1">
-        <v>2239</v>
+      <c r="C99" s="1" t="s">
+        <v>515</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>548</v>
+        <v>571</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>548</v>
+        <v>571</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>15</v>
@@ -4998,28 +5013,28 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>750100075</v>
+        <v>750100042</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>179</v>
+        <v>9</v>
+      </c>
+      <c r="C100" s="1">
+        <v>2239</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>180</v>
+        <v>519</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>181</v>
+        <v>520</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>182</v>
+        <v>521</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>183</v>
+        <v>571</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>184</v>
+        <v>571</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>15</v>
@@ -5032,14 +5047,14 @@
       <c r="B101" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C101" s="1">
-        <v>1029</v>
+      <c r="C101" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>182</v>
@@ -5056,28 +5071,28 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>750100042</v>
+        <v>750100075</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>315</v>
+        <v>19</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1029</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>316</v>
+        <v>185</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>317</v>
+        <v>186</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>318</v>
+        <v>182</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>557</v>
+        <v>183</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>319</v>
+        <v>184</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>15</v>
@@ -5091,19 +5106,19 @@
         <v>9</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>319</v>
@@ -5120,22 +5135,22 @@
         <v>9</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>384</v>
+        <v>320</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>45</v>
+        <v>321</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>385</v>
+        <v>322</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>386</v>
+        <v>323</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>387</v>
+        <v>556</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>387</v>
+        <v>319</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>15</v>
@@ -5148,23 +5163,23 @@
       <c r="B105" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="1">
-        <v>2321</v>
+      <c r="C105" s="1" t="s">
+        <v>384</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>324</v>
+        <v>45</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>325</v>
+        <v>385</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>326</v>
+        <v>386</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>556</v>
+        <v>387</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>327</v>
+        <v>387</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>15</v>
@@ -5178,19 +5193,19 @@
         <v>9</v>
       </c>
       <c r="C106" s="1">
-        <v>1904</v>
+        <v>2321</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>327</v>
@@ -5207,19 +5222,19 @@
         <v>9</v>
       </c>
       <c r="C107" s="1">
-        <v>2036</v>
+        <v>1904</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>327</v>
@@ -5236,19 +5251,19 @@
         <v>9</v>
       </c>
       <c r="C108" s="1">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>327</v>
@@ -5264,20 +5279,20 @@
       <c r="B109" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>388</v>
+      <c r="C109" s="1">
+        <v>2037</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>47</v>
+        <v>344</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>389</v>
+        <v>345</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>390</v>
+        <v>346</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>327</v>
@@ -5288,28 +5303,28 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>750100075</v>
+        <v>750100042</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>20</v>
+        <v>388</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>22</v>
+        <v>389</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>23</v>
+        <v>390</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>564</v>
+        <v>327</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>15</v>
@@ -5322,23 +5337,23 @@
       <c r="B111" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C111" s="1">
-        <v>1032</v>
+      <c r="C111" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>15</v>
@@ -5352,22 +5367,22 @@
         <v>19</v>
       </c>
       <c r="C112" s="1">
-        <v>2032</v>
+        <v>1032</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>15</v>
@@ -5375,28 +5390,28 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>750100042</v>
+        <v>750100075</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>331</v>
+        <v>19</v>
+      </c>
+      <c r="C113" s="1">
+        <v>2032</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>332</v>
+        <v>27</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>333</v>
+        <v>28</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>334</v>
+        <v>29</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>335</v>
+        <v>564</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>335</v>
+        <v>564</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>15</v>
@@ -5410,19 +5425,19 @@
         <v>9</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>335</v>
@@ -5439,25 +5454,25 @@
         <v>9</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>489</v>
+        <v>336</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>161</v>
+        <v>337</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>490</v>
+        <v>338</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>491</v>
+        <v>339</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>492</v>
+        <v>340</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>493</v>
+        <v>335</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>309</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -5467,14 +5482,14 @@
       <c r="B116" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C116" s="1">
-        <v>1535</v>
+      <c r="C116" s="1" t="s">
+        <v>489</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>491</v>
@@ -5496,23 +5511,23 @@
       <c r="B117" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>305</v>
+      <c r="C117" s="1">
+        <v>1535</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>306</v>
+        <v>494</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>307</v>
+        <v>491</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>308</v>
+        <v>492</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>308</v>
+        <v>493</v>
       </c>
       <c r="I117" s="1" t="s">
         <v>309</v>
@@ -5526,16 +5541,16 @@
         <v>9</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>308</v>
@@ -5554,17 +5569,17 @@
       <c r="B119" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C119" s="1">
-        <v>1361</v>
+      <c r="C119" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>313</v>
+        <v>16</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>308</v>
@@ -5584,25 +5599,25 @@
         <v>9</v>
       </c>
       <c r="C120" s="1">
-        <v>2238</v>
+        <v>1361</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>482</v>
+        <v>313</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>483</v>
+        <v>314</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>484</v>
+        <v>307</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>552</v>
+        <v>308</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>349</v>
+        <v>308</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>350</v>
+        <v>309</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -5613,22 +5628,22 @@
         <v>9</v>
       </c>
       <c r="C121" s="1">
-        <v>2248</v>
+        <v>2238</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>428</v>
+        <v>482</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>429</v>
+        <v>483</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>430</v>
+        <v>484</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>431</v>
+        <v>551</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>422</v>
+        <v>349</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>350</v>
@@ -5642,22 +5657,22 @@
         <v>9</v>
       </c>
       <c r="C122" s="1">
-        <v>2247</v>
+        <v>2248</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>485</v>
+        <v>428</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>486</v>
+        <v>429</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>487</v>
+        <v>430</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>431</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>488</v>
+        <v>422</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>350</v>
@@ -5671,22 +5686,22 @@
         <v>9</v>
       </c>
       <c r="C123" s="1">
-        <v>1362</v>
+        <v>2247</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>361</v>
+        <v>485</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>362</v>
+        <v>486</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>363</v>
+        <v>487</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>364</v>
+        <v>431</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>349</v>
+        <v>488</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>350</v>
@@ -5700,16 +5715,16 @@
         <v>9</v>
       </c>
       <c r="C124" s="1">
-        <v>1472</v>
+        <v>1362</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>364</v>
@@ -5729,16 +5744,16 @@
         <v>9</v>
       </c>
       <c r="C125" s="1">
-        <v>1363</v>
+        <v>1472</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>364</v>
@@ -5758,13 +5773,13 @@
         <v>9</v>
       </c>
       <c r="C126" s="1">
-        <v>1524</v>
+        <v>1363</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>364</v>
@@ -5786,23 +5801,23 @@
       <c r="B127" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>501</v>
+      <c r="C127" s="1">
+        <v>1524</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>180</v>
+        <v>370</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>502</v>
+        <v>371</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>503</v>
+        <v>364</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>553</v>
+        <v>364</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>504</v>
+        <v>349</v>
       </c>
       <c r="I127" s="1" t="s">
         <v>350</v>
@@ -5815,20 +5830,20 @@
       <c r="B128" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C128" s="1">
-        <v>1974</v>
+      <c r="C128" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>503</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>504</v>
@@ -5845,22 +5860,22 @@
         <v>9</v>
       </c>
       <c r="C129" s="1">
-        <v>2480</v>
+        <v>1974</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>506</v>
+        <v>185</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>509</v>
+        <v>552</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>350</v>
@@ -5874,16 +5889,16 @@
         <v>9</v>
       </c>
       <c r="C130" s="1">
-        <v>2485</v>
+        <v>2480</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>205</v>
+        <v>506</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>509</v>
@@ -5903,22 +5918,22 @@
         <v>9</v>
       </c>
       <c r="C131" s="1">
-        <v>2030</v>
+        <v>2485</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>27</v>
+        <v>205</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>354</v>
+        <v>511</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>355</v>
+        <v>512</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>355</v>
+        <v>509</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>349</v>
+        <v>510</v>
       </c>
       <c r="I131" s="1" t="s">
         <v>350</v>
@@ -5931,20 +5946,20 @@
       <c r="B132" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>356</v>
+      <c r="C132" s="1">
+        <v>2030</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>357</v>
+        <v>27</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>349</v>
@@ -5961,22 +5976,22 @@
         <v>9</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>420</v>
+        <v>356</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>65</v>
+        <v>357</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>421</v>
+        <v>358</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>422</v>
+        <v>359</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>422</v>
+        <v>360</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>422</v>
+        <v>349</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>350</v>
@@ -5990,19 +6005,19 @@
         <v>9</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>424</v>
+        <v>65</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>422</v>
@@ -6018,17 +6033,17 @@
       <c r="B135" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C135" s="1">
-        <v>1364</v>
+      <c r="C135" s="1" t="s">
+        <v>423</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>427</v>
@@ -6047,23 +6062,23 @@
       <c r="B136" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>347</v>
+      <c r="C136" s="1">
+        <v>1364</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>21</v>
+        <v>432</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>348</v>
+        <v>433</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>349</v>
+        <v>422</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>349</v>
+        <v>427</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>349</v>
+        <v>422</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>350</v>
@@ -6077,16 +6092,16 @@
         <v>9</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>349</v>
@@ -6106,22 +6121,22 @@
         <v>9</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>441</v>
+        <v>351</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>442</v>
+        <v>24</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>443</v>
+        <v>352</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>444</v>
+        <v>353</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>444</v>
+        <v>349</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>444</v>
+        <v>349</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>350</v>
@@ -6134,17 +6149,17 @@
       <c r="B139" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C139" s="1">
-        <v>1534</v>
+      <c r="C139" s="1" t="s">
+        <v>441</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>444</v>
@@ -6164,16 +6179,16 @@
         <v>9</v>
       </c>
       <c r="C140" s="1">
-        <v>2464</v>
+        <v>1534</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>444</v>
@@ -6192,23 +6207,23 @@
       <c r="B141" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>434</v>
+      <c r="C141" s="1">
+        <v>2464</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>436</v>
+        <v>449</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>76</v>
+        <v>450</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>76</v>
+        <v>444</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>76</v>
+        <v>444</v>
       </c>
       <c r="I141" s="1" t="s">
         <v>350</v>
@@ -6221,14 +6236,14 @@
       <c r="B142" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C142" s="1">
-        <v>1533</v>
+      <c r="C142" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>76</v>
@@ -6251,13 +6266,13 @@
         <v>9</v>
       </c>
       <c r="C143" s="1">
-        <v>2506</v>
+        <v>1533</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>76</v>
@@ -6280,16 +6295,16 @@
         <v>9</v>
       </c>
       <c r="C144" s="1">
-        <v>1973</v>
+        <v>2506</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>495</v>
+        <v>439</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>496</v>
+        <v>440</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>497</v>
+        <v>76</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>76</v>
@@ -6309,16 +6324,16 @@
         <v>9</v>
       </c>
       <c r="C145" s="1">
-        <v>1985</v>
+        <v>1973</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="G145" s="1" t="s">
         <v>76</v>
@@ -6337,26 +6352,26 @@
       <c r="B146" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>372</v>
+      <c r="C146" s="1">
+        <v>1985</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>373</v>
+        <v>498</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>374</v>
+        <v>499</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>375</v>
+        <v>500</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>375</v>
+        <v>76</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>375</v>
+        <v>76</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>85</v>
+        <v>350</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -6367,16 +6382,16 @@
         <v>9</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>375</v>
@@ -6396,19 +6411,19 @@
         <v>9</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>375</v>
@@ -6419,28 +6434,28 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>750100075</v>
+        <v>750100042</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C149" s="1">
-        <v>1469</v>
+        <v>9</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>380</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>103</v>
+        <v>381</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>104</v>
+        <v>382</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>105</v>
+        <v>383</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>562</v>
+        <v>383</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>562</v>
+        <v>375</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>85</v>
@@ -6454,22 +6469,22 @@
         <v>19</v>
       </c>
       <c r="C150" s="1">
-        <v>1421</v>
+        <v>1469</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>85</v>
@@ -6483,22 +6498,22 @@
         <v>19</v>
       </c>
       <c r="C151" s="1">
-        <v>2555</v>
+        <v>1421</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>85</v>
@@ -6506,28 +6521,28 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>750100042</v>
+        <v>750100075</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>470</v>
+        <v>19</v>
+      </c>
+      <c r="C152" s="1">
+        <v>2555</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>471</v>
+        <v>109</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>472</v>
+        <v>110</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>473</v>
+        <v>108</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="I152" s="1" t="s">
         <v>85</v>
@@ -6540,23 +6555,23 @@
       <c r="B153" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C153" s="1">
-        <v>2358</v>
+      <c r="C153" s="1" t="s">
+        <v>470</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>476</v>
+        <v>549</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I153" s="1" t="s">
         <v>85</v>
@@ -6569,23 +6584,23 @@
       <c r="B154" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>451</v>
+      <c r="C154" s="1">
+        <v>2358</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>73</v>
+        <v>474</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>452</v>
+        <v>475</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>454</v>
+        <v>476</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>84</v>
+        <v>550</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>85</v>
@@ -6598,17 +6613,17 @@
       <c r="B155" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C155" s="1">
-        <v>2483</v>
+      <c r="C155" s="1" t="s">
+        <v>451</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>455</v>
+        <v>73</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>454</v>
@@ -6622,25 +6637,25 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>750100075</v>
+        <v>750100042</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
+      </c>
+      <c r="C156" s="1">
+        <v>2483</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>81</v>
+        <v>455</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>82</v>
+        <v>456</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>83</v>
+        <v>457</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>544</v>
+        <v>454</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>84</v>
@@ -6657,16 +6672,16 @@
         <v>19</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>540</v>
+        <v>80</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>541</v>
+        <v>81</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>542</v>
+        <v>82</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>543</v>
+        <v>83</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>544</v>
@@ -6686,13 +6701,13 @@
         <v>19</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="D158" s="1">
-        <v>545</v>
-      </c>
-      <c r="E158" s="1">
-        <v>76545</v>
+        <v>540</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>542</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>543</v>
@@ -6709,30 +6724,59 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>750100042</v>
+        <v>750100075</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C159" s="1">
+        <v>19</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D159" s="1">
+        <v>545</v>
+      </c>
+      <c r="E159" s="1">
+        <v>76545</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="G159" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="H159" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I159" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>750100042</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C160" s="1">
         <v>2543</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="D160" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="E159" s="1" t="s">
+      <c r="E160" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="F159" s="1" t="s">
+      <c r="F160" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="G159" s="1" t="s">
+      <c r="G160" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="H159" s="1" t="s">
+      <c r="H160" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="I159" s="1" t="s">
+      <c r="I160" s="1" t="s">
         <v>481</v>
       </c>
     </row>

</xml_diff>